<commit_message>
Alter the database mode(20160426_v1)
</commit_message>
<xml_diff>
--- a/AbkSection/UI2/reportData.xlsx
+++ b/AbkSection/UI2/reportData.xlsx
@@ -19,7 +19,7 @@
     <t>ID:</t>
   </si>
   <si>
-    <t>20160421163554</t>
+    <t>20160425144344</t>
   </si>
   <si>
     <t>Area:</t>
@@ -43,13 +43,13 @@
     <t>centroid</t>
   </si>
   <si>
-    <t>[0.9166666666666667, 1.9166666666666667]</t>
+    <t>[0.0, 0.0]</t>
   </si>
   <si>
     <t>tan_alfa</t>
   </si>
   <si>
-    <t>0.25510259478</t>
+    <t>pi/4</t>
   </si>
   <si>
     <t>ix</t>
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>11.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>5.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -477,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>29.25</v>
+        <v>725.333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>7.25</v>
+        <v>725.333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -493,7 +493,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>9.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -517,7 +517,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>3.00061888459431</v>
+        <v>3.36650164612069</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -525,7 +525,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>1.11386753864619</v>
+        <v>3.36650164612069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>